<commit_message>
Feito do Exercício 3 ao 5
</commit_message>
<xml_diff>
--- a/Exercicios_CSharp.xlsx
+++ b/Exercicios_CSharp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pointcondominio-my.sharepoint.com/personal/eric_silva_pointcondominio_onmicrosoft_com/Documents/Área de Trabalho/Codigos/C#/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB2AB491-045B-4B4E-AE3A-D288C1495533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{DB2AB491-045B-4B4E-AE3A-D288C1495533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1CCDF81-B411-4D21-BB4A-A35E367BDEE4}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +615,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Feito Exercicio 10, acabado Exercicios básicos
</commit_message>
<xml_diff>
--- a/Exercicios_CSharp.xlsx
+++ b/Exercicios_CSharp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pointcondominio-my.sharepoint.com/personal/eric_silva_pointcondominio_onmicrosoft_com/Documents/Área de Trabalho/Codigos/C#/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{DB2AB491-045B-4B4E-AE3A-D288C1495533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7DD03B7-4660-4EB9-AC38-D734CB56C54A}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{DB2AB491-045B-4B4E-AE3A-D288C1495533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14A48287-4F7A-4A6D-A478-3AD7EBE378D2}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -594,7 +594,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,8 +717,8 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="b">
-        <v>0</v>
+      <c r="C11" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>